<commit_message>
Added _TULOS to result file name AND added Tunniste-field
</commit_message>
<xml_diff>
--- a/excel_templates/katuosoitteilla.xlsx
+++ b/excel_templates/katuosoitteilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyrki.jylha\vkm-ui-legacy\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF818E6-C9CC-44A5-B068-DF9485227324}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9518F383-C17A-425C-9A01-47107A9246C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="1680" windowWidth="25455" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Kunta</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Katunimi</t>
+  </si>
+  <si>
+    <t>Tunniste</t>
   </si>
 </sst>
 </file>
@@ -383,13 +386,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -399,6 +404,9 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>